<commit_message>
Check for full feeds
</commit_message>
<xml_diff>
--- a/data/_general_data/diets/all_feeds.xlsx
+++ b/data/_general_data/diets/all_feeds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treimer\Documents\R-temp-files\local_to_global_mariculture_modelling\data\_general_data\diets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABC58F6-1D4D-448D-BBA7-525DAFC5E7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869C39F4-483E-4F83-B717-0DB9D35AF2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="1356" windowWidth="16860" windowHeight="14664" activeTab="1" xr2:uid="{A3945701-1F25-4092-97C8-50D4B2B937C4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{A3945701-1F25-4092-97C8-50D4B2B937C4}"/>
   </bookViews>
   <sheets>
     <sheet name="all_feeds" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>ingredient</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>coconut-oil</t>
-  </si>
-  <si>
-    <t>corn-gluten-meal</t>
   </si>
   <si>
     <t>faba-beans</t>
@@ -3044,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76559CA1-42BE-4BD5-A831-409A491DC0E7}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3128,7 +3125,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>7.0000000000000001E-3</v>
@@ -3142,7 +3139,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>3.5999999999999997E-2</v>
@@ -3156,7 +3153,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>8.7999999999999995E-2</v>
@@ -3170,7 +3167,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>3.3000000000000002E-2</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>8.4000000000000005E-2</v>
@@ -3198,7 +3195,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>0.02</v>
@@ -3212,7 +3209,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>4.2999999999999997E-2</v>
@@ -3226,7 +3223,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>4.0000000000000001E-3</v>
@@ -3240,7 +3237,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>1.2999999999999999E-2</v>
@@ -3254,7 +3251,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3268,7 +3265,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>2.5000000000000001E-2</v>
@@ -3282,7 +3279,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>1.4E-2</v>
@@ -3296,7 +3293,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3310,7 +3307,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>4.0000000000000001E-3</v>
@@ -3324,7 +3321,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>0.20899999999999999</v>
@@ -3338,7 +3335,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3352,7 +3349,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>3.4000000000000002E-2</v>
@@ -3366,7 +3363,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>6.5000000000000002E-2</v>
@@ -3380,7 +3377,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>9.8000000000000004E-2</v>
@@ -3394,15 +3391,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>4.1000000000000002E-2</v>
       </c>
+      <c r="C25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D25">
+        <v>4.1000000000000002E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3423,8 +3426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E575356-B323-4D16-82DC-0AC8D69C8CE8}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3438,24 +3441,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3472,10 +3475,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -3489,7 +3492,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -3506,7 +3509,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3523,7 +3526,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -3540,10 +3543,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>7.6616313903328332E-3</v>
@@ -3557,10 +3560,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>2.1556568613219654E-2</v>
@@ -3574,10 +3577,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
         <v>0.14871006944806647</v>
@@ -3592,10 +3595,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>4.5596717977033734E-2</v>
@@ -3609,10 +3612,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>8.7076221638678522E-2</v>
@@ -3626,10 +3629,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
         <v>2.4751502209397133E-2</v>
@@ -3643,10 +3646,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -3661,10 +3664,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -3678,10 +3681,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -3697,10 +3700,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -3715,10 +3718,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -3732,10 +3735,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -3749,10 +3752,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
         <v>3.1062405944578275E-2</v>
@@ -3766,10 +3769,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>1.0085252416118028E-2</v>
@@ -3783,10 +3786,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>7.9231644148489502E-3</v>
@@ -3800,10 +3803,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1">
         <v>0.18312885370749094</v>
@@ -3817,10 +3820,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -3834,10 +3837,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -3851,10 +3854,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -3868,10 +3871,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1">
         <v>0.21236849084420042</v>
@@ -3885,10 +3888,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -3902,10 +3905,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -3919,10 +3922,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1">
         <v>5.9628304610637353E-2</v>
@@ -3936,10 +3939,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="1">
         <v>2.0800144057534814E-3</v>
@@ -3953,10 +3956,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1">
         <v>9.8875407994580694E-2</v>
@@ -3970,10 +3973,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="1">
         <v>5.9495394385063585E-2</v>
@@ -3987,10 +3990,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -4030,27 +4033,27 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4070,7 +4073,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0.30613451127317587</v>
@@ -4090,7 +4093,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4110,7 +4113,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>3.1062405944578275E-2</v>
@@ -4130,7 +4133,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>0.60317477817160847</v>
@@ -4150,7 +4153,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>0.94037169538936261</v>

</xml_diff>

<commit_message>
Updates to feeds documentation
</commit_message>
<xml_diff>
--- a/data/_general_data/diets/all_feeds.xlsx
+++ b/data/_general_data/diets/all_feeds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treimer\Documents\R-temp-files\local_to_global_mariculture_modelling\data\_general_data\diets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A0E2CF-A22C-45AE-A7B5-DCE5286D5241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E302938D-2E4C-4FFC-8D8C-47E97FCDA3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A3945701-1F25-4092-97C8-50D4B2B937C4}"/>
+    <workbookView xWindow="15252" yWindow="1500" windowWidth="22884" windowHeight="14232" xr2:uid="{A3945701-1F25-4092-97C8-50D4B2B937C4}"/>
   </bookViews>
   <sheets>
     <sheet name="all_feeds" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,9 @@
     <author>tc={450A82A6-3C86-498F-ACC8-26ADEC349CDC}</author>
     <author>tc={295CEF34-0691-49CD-B4AA-404CFA1941B5}</author>
     <author>tc={6F58248A-EEB9-408F-A011-550C259F83D1}</author>
-    <author>tc={66269F61-1EA7-4522-A6E8-C17271CC498A}</author>
     <author>tc={202B778C-4D59-41E3-B4D4-415CB93CFCBA}</author>
     <author>tc={A52D0341-65F2-4636-B34E-E5D8EBC0680B}</author>
+    <author>tc={66269F61-1EA7-4522-A6E8-C17271CC498A}</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{0C425B69-1EAF-4622-ABE6-30EE0C7BDD5F}">
@@ -97,15 +97,7 @@
     From Tom Fox-Smith, representative of a higher animal ingredient inclusion</t>
       </text>
     </comment>
-    <comment ref="E3" authorId="6" shapeId="0" xr:uid="{66269F61-1EA7-4522-A6E8-C17271CC498A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Tom’s formulation lumps fishmeal and krill altogether at 40%.</t>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="7" shapeId="0" xr:uid="{202B778C-4D59-41E3-B4D4-415CB93CFCBA}">
+    <comment ref="B9" authorId="6" shapeId="0" xr:uid="{202B778C-4D59-41E3-B4D4-415CB93CFCBA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -113,12 +105,20 @@
     From Ytrestøyl (2015) Figure 2, average of 25.2% of marine ingredients are from trimmings from years 2010-2013.</t>
       </text>
     </comment>
-    <comment ref="B10" authorId="8" shapeId="0" xr:uid="{A52D0341-65F2-4636-B34E-E5D8EBC0680B}">
+    <comment ref="B11" authorId="7" shapeId="0" xr:uid="{A52D0341-65F2-4636-B34E-E5D8EBC0680B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     From Ytrestøyl (2015) Figure 2, average of 25.2% of marine ingredients are from trimmings from years 2010-2013.</t>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="8" shapeId="0" xr:uid="{66269F61-1EA7-4522-A6E8-C17271CC498A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tom’s formulation lumps fishmeal and krill altogether at 40%.</t>
       </text>
     </comment>
   </commentList>
@@ -1152,14 +1152,14 @@
   <threadedComment ref="G1" dT="2025-11-27T00:03:37.69" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{6F58248A-EEB9-408F-A011-550C259F83D1}">
     <text>From Tom Fox-Smith, representative of a higher animal ingredient inclusion</text>
   </threadedComment>
-  <threadedComment ref="E3" dT="2025-11-26T23:56:58.41" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{66269F61-1EA7-4522-A6E8-C17271CC498A}">
-    <text>Tom’s formulation lumps fishmeal and krill altogether at 40%.</text>
-  </threadedComment>
-  <threadedComment ref="B6" dT="2025-11-26T23:39:37.94" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{202B778C-4D59-41E3-B4D4-415CB93CFCBA}">
+  <threadedComment ref="B9" dT="2025-11-26T23:39:37.94" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{202B778C-4D59-41E3-B4D4-415CB93CFCBA}">
     <text>From Ytrestøyl (2015) Figure 2, average of 25.2% of marine ingredients are from trimmings from years 2010-2013.</text>
   </threadedComment>
-  <threadedComment ref="B10" dT="2025-11-26T23:39:37.94" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{A52D0341-65F2-4636-B34E-E5D8EBC0680B}">
+  <threadedComment ref="B11" dT="2025-11-26T23:39:37.94" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{A52D0341-65F2-4636-B34E-E5D8EBC0680B}">
     <text>From Ytrestøyl (2015) Figure 2, average of 25.2% of marine ingredients are from trimmings from years 2010-2013.</text>
+  </threadedComment>
+  <threadedComment ref="E21" dT="2025-11-26T23:56:58.41" personId="{CF1D84E9-9E0E-47B8-AF49-4AA23DD844A8}" id="{66269F61-1EA7-4522-A6E8-C17271CC498A}">
+    <text>Tom’s formulation lumps fishmeal and krill altogether at 40%.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1170,7 +1170,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,515 +1209,518 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.183</v>
-      </c>
-      <c r="C2" s="1">
-        <f>18%+0.4%</f>
-        <v>0.184</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1">
-        <v>0.14605647517039919</v>
+        <v>0.02</v>
       </c>
       <c r="E2" s="1">
-        <v>0.23649999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="F2" s="1">
-        <v>0.24079999999999999</v>
+        <f>7.5%*0.25</f>
+        <v>1.8749999999999999E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>0.1008</v>
+        <f>7.5%*0.25</f>
+        <v>1.8749999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <f>19.5*(1-0.252)%</f>
-        <v>0.14585999999999999</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
-        <f>30*0.75%</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="F3" s="1">
-        <f>7.5%*0.75*0.75</f>
-        <v>4.2187499999999996E-2</v>
-      </c>
-      <c r="G3" s="1">
-        <f>7.5%*0.75*0.75</f>
-        <v>4.2187499999999996E-2</v>
-      </c>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.9000000000000005E-2</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>0.2087</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.1077</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.1242</v>
-      </c>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3.1E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
       <c r="D5" s="1">
-        <v>1.9474196689386561E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E5" s="1">
-        <v>0.1</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="F5" s="1">
-        <f>7.5%*0.25</f>
-        <v>1.8749999999999999E-2</v>
+        <v>2.76E-2</v>
       </c>
       <c r="G5" s="1">
-        <f>7.5%*0.25</f>
-        <v>1.8749999999999999E-2</v>
+        <v>1.12E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>2.69E-2</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B9" s="1">
         <f>19.5*0.252%</f>
         <v>4.9140000000000003E-2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C9" s="1">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="D6" s="1">
-        <v>4.8685491723466402E-2</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D9" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E9" s="1">
         <f>30*0.25%</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F9" s="1">
         <f>7.5%*0.75*0.25</f>
         <v>1.4062499999999999E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G9" s="1">
         <f>7.5%*0.75*0.25</f>
         <v>1.4062499999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <f>11.2*(1-0.252)%</f>
-        <v>8.3775999999999989E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.9474196689386561E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <f>7.69*0.75%</f>
-        <v>5.7675000000000004E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <f>4.54%*0.75</f>
-        <v>3.4050000000000004E-2</v>
-      </c>
-      <c r="G7" s="1">
-        <f>6.12%*0.75</f>
-        <v>4.5900000000000003E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1">
-        <v>3.78E-2</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1">
-        <v>0.26840000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>1.7100000000000001E-2</v>
-      </c>
-    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <f>11.2*0.252%</f>
         <v>2.8223999999999999E-2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>0.02</v>
       </c>
-      <c r="D10" s="1">
-        <v>4.8685491723466402E-2</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="D11" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E11" s="1">
         <f>7.69*0.25%</f>
         <v>1.9225000000000003E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <f>4.54%*0.25</f>
         <v>1.1350000000000001E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G11" s="1">
         <f>6.12%*0.25</f>
         <v>1.5300000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3.1E-2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4.5764362220058419E-2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.76E-2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1.12E-2</v>
-      </c>
-    </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.8800000000000001E-2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>2.7000000000000001E-3</v>
-      </c>
+      <c r="C12" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>0.08</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1">
-        <v>0.11849999999999999</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7.0000000000000001E-3</v>
+      </c>
       <c r="D15" s="1">
-        <v>9.7370983446932804E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1">
-        <v>0.05</v>
-      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.125</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
-        <v>4.7600000000000003E-2</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.04</v>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.183</v>
+      </c>
+      <c r="C17" s="1">
+        <f>18%+0.4%</f>
+        <v>0.184</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.185</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.23649999999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.24079999999999999</v>
+      </c>
       <c r="G17" s="1">
-        <v>1.83E-2</v>
+        <v>0.1008</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>0.15</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.14605647517039919</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <v>2.5999999999999999E-3</v>
+      </c>
       <c r="F19" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1">
-        <v>5.8000000000000003E-2</v>
+        <f>11.2*(1-0.252)%</f>
+        <v>8.3775999999999989E-2</v>
       </c>
       <c r="C20" s="1">
-        <v>9.8000000000000004E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <f>7.69*0.75%</f>
+        <v>5.7675000000000004E-2</v>
+      </c>
       <c r="F20" s="1">
-        <v>9.74E-2</v>
-      </c>
-      <c r="G20" s="1"/>
+        <f>4.54%*0.75</f>
+        <v>3.4050000000000004E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <f>6.12%*0.75</f>
+        <v>4.5900000000000003E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
-        <v>8.0000000000000002E-3</v>
+        <f>19.5*(1-0.252)%</f>
+        <v>0.14585999999999999</v>
       </c>
       <c r="C21" s="1">
-        <v>1.4E-2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>4.8685491723466402E-2</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <f>30*0.75%</f>
+        <v>0.22499999999999998</v>
+      </c>
       <c r="F21" s="1">
-        <v>2.69E-2</v>
-      </c>
-      <c r="G21" s="1"/>
+        <f>7.5%*0.75*0.75</f>
+        <v>4.2187499999999996E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <f>7.5%*0.75*0.75</f>
+        <v>4.2187499999999996E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1">
-        <v>4.8685491723466402E-2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1">
+        <v>9.74E-2</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="E24" s="1">
+        <v>0.2087</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.1077</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.1242</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="1">
-        <v>1E-3</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1">
+        <v>0.15</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C26" s="1">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D26" s="1">
-        <v>7.7896786757546244E-2</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
+        <v>3.78E-2</v>
+      </c>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1">
+        <v>0.26840000000000003</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="1">
-        <f>1.9%+0.3%</f>
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3.5999999999999997E-2</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>2.6599999999999999E-2</v>
+      </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <v>1.7100000000000001E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="1">
-        <v>4.2999999999999997E-2</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>0.11849999999999999</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="1">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.9211295034079838E-2</v>
-      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1">
+        <v>1.83E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1725,10 +1728,12 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="1">
+        <v>1E-3</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1736,25 +1741,28 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B33" s="1">
+        <f>1.9%+0.3%</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
       <c r="C33" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D33" s="1">
-        <v>6.815968841285297E-2</v>
-      </c>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1">
+        <v>4.2999999999999997E-2</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1762,42 +1770,36 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1.9474196689386561E-2</v>
-      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1">
-        <v>6.815968841285297E-2</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3.4000000000000002E-2</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1805,7 +1807,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1816,12 +1818,14 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B39" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1829,19 +1833,21 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1">
-        <v>6.815968841285297E-2</v>
-      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G40" xr:uid="{76559CA1-42BE-4BD5-A831-409A491DC0E7}"/>
+  <autoFilter ref="A1:G40" xr:uid="{76559CA1-42BE-4BD5-A831-409A491DC0E7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G40">
+      <sortCondition ref="D1:D40"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>